<commit_message>
songs to radio level
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut2.xlsx
+++ b/core/assets/levels/tut2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5AD4EC-AC6E-49ED-8F58-DAE2A1BE20D5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D349F5-F5D8-4703-A6A5-B797F6E90733}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Region</t>
   </si>
@@ -300,6 +300,30 @@
   </si>
   <si>
     <t>* tell them to switch channel</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Classical</t>
+  </si>
+  <si>
+    <t>rustling_leaves.mp3</t>
+  </si>
+  <si>
+    <t>bensound-extremeaction.mp3</t>
+  </si>
+  <si>
+    <t>bensound-countryboy.mp3</t>
+  </si>
+  <si>
+    <t>bensound-dance.mp3</t>
+  </si>
+  <si>
+    <t>Dance</t>
   </si>
 </sst>
 </file>
@@ -720,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -876,6 +900,12 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="G9" s="11"/>
@@ -883,6 +913,12 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="G10" s="11"/>
@@ -890,6 +926,12 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" t="s">
@@ -900,8 +942,12 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="G12" s="11"/>

</xml_diff>

<commit_message>
radio show like/dislike, classical always first channel
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut2.xlsx
+++ b/core/assets/levels/tut2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D349F5-F5D8-4703-A6A5-B797F6E90733}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD410745-E11B-43B5-B4F1-2AC947890109}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8745" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,25 +305,25 @@
     <t>Pop</t>
   </si>
   <si>
-    <t>Action</t>
-  </si>
-  <si>
     <t>Classical</t>
   </si>
   <si>
     <t>rustling_leaves.mp3</t>
   </si>
   <si>
-    <t>bensound-extremeaction.mp3</t>
-  </si>
-  <si>
-    <t>bensound-countryboy.mp3</t>
-  </si>
-  <si>
     <t>bensound-dance.mp3</t>
   </si>
   <si>
-    <t>Dance</t>
+    <t>Comedy</t>
+  </si>
+  <si>
+    <t>bensound-funkyelement.mp3</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>bensound-jazzyfrenchy.mp3</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
   <dimension ref="A1:AS1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -900,24 +900,22 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A9" t="s">
-        <v>50</v>
+      <c r="A9" s="2" t="s">
+        <v>51</v>
       </c>
-      <c r="B9" t="s">
-        <v>56</v>
+      <c r="B9" s="2" t="s">
+        <v>52</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
       <c r="G9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -927,10 +925,10 @@
     </row>
     <row r="11" spans="1:11" ht="16.5" customHeight="1">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -942,10 +940,10 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>52</v>
+      <c r="A12" t="s">
+        <v>50</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="2"/>

</xml_diff>

<commit_message>
don't change the tuts or levels lol
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut2.xlsx
+++ b/core/assets/levels/tut2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A064D0A1-77A1-4D25-919E-8C03661CFB23}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8313CB1C-1C60-4DFE-9D52-556EDC0175B7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9690" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -299,9 +299,6 @@
     <t>Classical</t>
   </si>
   <si>
-    <t>rustling_leaves.mp3</t>
-  </si>
-  <si>
     <t>bensound-dance.mp3</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>bensound-jazzyfrenchy.mp3</t>
+  </si>
+  <si>
+    <t>bensound-ofeliasdream.mp3</t>
   </si>
 </sst>
 </file>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -895,7 +895,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G9" s="11"/>
       <c r="I9" s="11"/>
@@ -903,10 +903,10 @@
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -916,10 +916,10 @@
     </row>
     <row r="11" spans="1:11" ht="16.5" customHeight="1">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -932,7 +932,7 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>

</xml_diff>